<commit_message>
Finished Spreadsheet, updated with all channels
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Inputs</t>
   </si>
@@ -44,27 +44,6 @@
     <t>Digital Input</t>
   </si>
   <si>
-    <t>GearGate</t>
-  </si>
-  <si>
-    <t>GearRail</t>
-  </si>
-  <si>
-    <t>TurretPosition</t>
-  </si>
-  <si>
-    <t>DriveSpeed</t>
-  </si>
-  <si>
-    <t>ShooterWheelSpeed</t>
-  </si>
-  <si>
-    <t>GearPegPosition</t>
-  </si>
-  <si>
-    <t>GearCollected</t>
-  </si>
-  <si>
     <t>Drive Motors</t>
   </si>
   <si>
@@ -74,45 +53,6 @@
     <t>Pneumatics</t>
   </si>
   <si>
-    <t>GearPusher(Dual)</t>
-  </si>
-  <si>
-    <t>GearChute(Dual)</t>
-  </si>
-  <si>
-    <t>Shifter(Dual)</t>
-  </si>
-  <si>
-    <t>LeftDriveFront (CAN)</t>
-  </si>
-  <si>
-    <t>LeftDriveBack (CAN)</t>
-  </si>
-  <si>
-    <t>RightDriveFront (CAN)</t>
-  </si>
-  <si>
-    <t>RightDriveBack (CAN)</t>
-  </si>
-  <si>
-    <t>Shooter (CAN)</t>
-  </si>
-  <si>
-    <t>ShooterFeeder (CAN)</t>
-  </si>
-  <si>
-    <t>GearRail (CAN)</t>
-  </si>
-  <si>
-    <t>GearGate (CAN)</t>
-  </si>
-  <si>
-    <t>Intake (CAN)</t>
-  </si>
-  <si>
-    <t>Climber (CAN)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -216,6 +156,72 @@
   </si>
   <si>
     <t>Climber Up</t>
+  </si>
+  <si>
+    <t>RightDriveFront CAN-1 PWM-3</t>
+  </si>
+  <si>
+    <t>LeftDriveMiddle CAN-N/A PWM-1</t>
+  </si>
+  <si>
+    <t>RightDriveMiddle CAN-N/A PWM-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeftDriveFront CAN-0 PWM-0  </t>
+  </si>
+  <si>
+    <t>LeftDriveBack CAN-2 PWM-2</t>
+  </si>
+  <si>
+    <t>RightDriveBack CAN-3 PWM-5</t>
+  </si>
+  <si>
+    <t>Shooter CAN-4 PWM-7</t>
+  </si>
+  <si>
+    <t>ShooterFeeder CAN-5 PWM-8</t>
+  </si>
+  <si>
+    <t>GearRail CAN-6 PWM-6</t>
+  </si>
+  <si>
+    <t>GearGate CAN-7 PWM-Invalid</t>
+  </si>
+  <si>
+    <t>Intake CAN-8 PWM-9</t>
+  </si>
+  <si>
+    <t>Climber CAN-9 PWM-Invalid</t>
+  </si>
+  <si>
+    <t>GearPusher(Dual) Solenoid 0, Solenoid 1</t>
+  </si>
+  <si>
+    <t>Shifter(Dual) Solenoid 2, Solenoid 3</t>
+  </si>
+  <si>
+    <t>GearChute(Dual) Solenoid 4, Solenoid 5</t>
+  </si>
+  <si>
+    <t>GearGate AI-0</t>
+  </si>
+  <si>
+    <t>GearRail AI-1</t>
+  </si>
+  <si>
+    <t>TurretPosition AI-2</t>
+  </si>
+  <si>
+    <t>DriveSpeed DIO-0,1</t>
+  </si>
+  <si>
+    <t>ShooterWheelSpeed DIO-2,3</t>
+  </si>
+  <si>
+    <t>GearPegPosition DIO-5</t>
+  </si>
+  <si>
+    <t>GearCollected DIO-6</t>
   </si>
 </sst>
 </file>
@@ -313,29 +319,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,6 +338,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,358 +633,365 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="B16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="1" t="s">
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="B20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="B22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="C25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added top roller control for feeder
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10848"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Inputs</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>GearCollected DIO-6</t>
+  </si>
+  <si>
+    <t>TopShooterMotor Can-11 PWM-Invalid</t>
+  </si>
+  <si>
+    <t>Ball_beambreak DIO-7</t>
   </si>
 </sst>
 </file>
@@ -633,22 +639,22 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" customWidth="1"/>
-    <col min="7" max="7" width="33.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -662,7 +668,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -686,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -710,7 +716,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -718,7 +724,9 @@
         <v>63</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" t="s">
         <v>45</v>
@@ -730,7 +738,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -748,7 +756,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -760,7 +768,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -772,7 +780,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -786,21 +794,24 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
@@ -811,7 +822,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -824,7 +835,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -838,7 +849,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -852,7 +863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -864,7 +875,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -878,7 +889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
@@ -892,7 +903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -906,7 +917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -920,7 +931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
@@ -932,7 +943,7 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
@@ -944,7 +955,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
@@ -958,7 +969,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -970,7 +981,7 @@
       </c>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -980,7 +991,7 @@
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Global Var setup completed still need to wire in periodic tasks
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Inputs</t>
   </si>
@@ -116,27 +116,18 @@
     <t>A</t>
   </si>
   <si>
-    <t>Shoot/Feed-F</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>Gear Gate Open</t>
   </si>
   <si>
-    <t>Gear Rail Right</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>Gear Gate Catch</t>
   </si>
   <si>
-    <t>Gear Rail Left</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>RB</t>
   </si>
   <si>
-    <t>Gear Pusher</t>
-  </si>
-  <si>
     <t>Feed Forward</t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t>LT</t>
   </si>
   <si>
-    <t>Climber Up</t>
-  </si>
-  <si>
     <t>Intake-B</t>
   </si>
   <si>
@@ -231,6 +216,24 @@
   </si>
   <si>
     <t>GearRail CAN-12 PWM-6</t>
+  </si>
+  <si>
+    <t>Shoot</t>
+  </si>
+  <si>
+    <t>Gear Rail Right/Left</t>
+  </si>
+  <si>
+    <t>GearPusher</t>
+  </si>
+  <si>
+    <t>BottomFeed Forward</t>
+  </si>
+  <si>
+    <t>BottomFeed Backward</t>
+  </si>
+  <si>
+    <t>Climb</t>
   </si>
 </sst>
 </file>
@@ -316,15 +319,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -348,6 +342,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,375 +633,373 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
-    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" customWidth="1"/>
+    <col min="9" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="4"/>
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+      <c r="G9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+      <c r="G10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-      <c r="G9" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="9"/>
-      <c r="G10" s="8" t="s">
+      <c r="C16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="11" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="B19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full manual control finished
that took longer than i expected...
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Inputs</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Shifter(Dual) Solenoid 2, Solenoid 3</t>
   </si>
   <si>
-    <t>GearGate CAN-7 PWM-Invalid</t>
-  </si>
-  <si>
     <t>RightDriveMiddle CAN-N/A PWM-4</t>
   </si>
   <si>
@@ -125,15 +122,9 @@
     <t>X</t>
   </si>
   <si>
-    <t>Gear Gate Catch</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Gear Gate Clamp</t>
-  </si>
-  <si>
     <t>RB</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Aim</t>
-  </si>
-  <si>
     <t>LS Y-Axis</t>
   </si>
   <si>
@@ -215,9 +203,6 @@
     <t>Shooter_Turret Can-10 PWM-Invalid</t>
   </si>
   <si>
-    <t>GearRail CAN-12 PWM-6</t>
-  </si>
-  <si>
     <t>Shoot</t>
   </si>
   <si>
@@ -234,6 +219,24 @@
   </si>
   <si>
     <t>Climb</t>
+  </si>
+  <si>
+    <t>Gear Gate Close</t>
+  </si>
+  <si>
+    <t>GearGate CAN-7 PWM-6</t>
+  </si>
+  <si>
+    <t>GearRail CAN-12 PWM-Invalid</t>
+  </si>
+  <si>
+    <t>Aim (still to do)</t>
+  </si>
+  <si>
+    <t>GearChute</t>
+  </si>
+  <si>
+    <t>PlaceGear</t>
   </si>
 </sst>
 </file>
@@ -633,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,10 +706,10 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>13</v>
@@ -728,7 +731,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>18</v>
@@ -746,7 +749,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>21</v>
@@ -757,10 +760,10 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -769,10 +772,10 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -783,10 +786,10 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -797,7 +800,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -807,199 +810,201 @@
       <c r="D10" s="4"/>
       <c r="E10" s="6"/>
       <c r="G10" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setup global vars and started work on setting up operator assist
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Inputs</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>PlaceGear</t>
+  </si>
+  <si>
+    <t>CollectGear</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +860,9 @@
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
cleaned and verified working
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Worked on finalizing Comp robot code, made gear place auto work
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Joysticks" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
   <si>
     <t>Pneumatics</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>2=Pusher</t>
+  </si>
+  <si>
+    <t>Joystick_DriveStraight</t>
   </si>
 </sst>
 </file>
@@ -501,17 +504,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,14 +816,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -856,7 +859,9 @@
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1020,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,20 +1040,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="10"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1057,7 +1062,7 @@
       <c r="B2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D2" t="s">
@@ -1081,7 +1086,7 @@
       <c r="B3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D3" t="s">
@@ -1105,7 +1110,7 @@
       <c r="B4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>124</v>
       </c>
       <c r="D4" t="s">
@@ -1128,7 +1133,7 @@
       <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D5" t="s">
@@ -1237,10 +1242,10 @@
       <c r="B11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="12"/>
       <c r="G11" t="s">
         <v>100</v>
       </c>
@@ -1272,10 +1277,10 @@
       <c r="E13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" t="s">

</xml_diff>

<commit_message>
Did Comp Robot checkout
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Joysticks" sheetId="1" r:id="rId1"/>
@@ -1082,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1801,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1992,10 +1992,10 @@
       </c>
       <c r="D14" s="20"/>
       <c r="H14" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -2005,10 +2005,10 @@
       <c r="C15" s="21"/>
       <c r="D15" s="20"/>
       <c r="H15" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2016,7 +2016,6 @@
       <c r="C16" s="21">
         <v>40</v>
       </c>
-      <c r="D16" s="20"/>
       <c r="H16" s="16" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
Real Competion Robot Testing
</commit_message>
<xml_diff>
--- a/IO_Claim_And_Joystick.xlsx
+++ b/IO_Claim_And_Joystick.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="6132" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Joysticks" sheetId="1" r:id="rId1"/>
     <sheet name="Robot IO" sheetId="2" r:id="rId2"/>
     <sheet name="Electrical Layout" sheetId="3" r:id="rId3"/>
+    <sheet name="Competition Robot Differences" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="171">
   <si>
     <t>Pneumatics</t>
   </si>
@@ -124,9 +125,6 @@
     <t>Climb</t>
   </si>
   <si>
-    <t>Gear Gate Close</t>
-  </si>
-  <si>
     <t>Aim (still to do)</t>
   </si>
   <si>
@@ -241,9 +239,6 @@
     <t>RightDriveBack</t>
   </si>
   <si>
-    <t>Shooter</t>
-  </si>
-  <si>
     <t>ShooterFeeder</t>
   </si>
   <si>
@@ -256,12 +251,6 @@
     <t>Climber</t>
   </si>
   <si>
-    <t>Shooter_Turret</t>
-  </si>
-  <si>
-    <t>TopShooterMotor</t>
-  </si>
-  <si>
     <t>GearRail</t>
   </si>
   <si>
@@ -430,9 +419,6 @@
     <t>3=Spare</t>
   </si>
   <si>
-    <t>New Setup</t>
-  </si>
-  <si>
     <t>Front</t>
   </si>
   <si>
@@ -518,13 +504,49 @@
   </si>
   <si>
     <t>Right Turret</t>
+  </si>
+  <si>
+    <t>Gear Gate Clamp</t>
+  </si>
+  <si>
+    <t>Implements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competition Robot </t>
+  </si>
+  <si>
+    <t>Practice Robot</t>
+  </si>
+  <si>
+    <t>Drive Speed</t>
+  </si>
+  <si>
+    <t>Gear Gate?</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Inverted</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Busted</t>
+  </si>
+  <si>
+    <t>Ehh…</t>
+  </si>
+  <si>
+    <t>Feeder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -547,6 +569,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -737,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -766,9 +794,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +825,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,14 +1134,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1130,13 +1164,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1144,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
@@ -1232,13 +1266,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1303,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1320,468 +1354,383 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="25"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="26"/>
+      <c r="G1" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>67</v>
+      <c r="A2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>68</v>
+      <c r="A3" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="E8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="8" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="E9" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="E10" s="7"/>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="G11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
       <c r="E14" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>134</v>
-      </c>
+      <c r="B15" s="11"/>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E15" s="8"/>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="E16" s="8"/>
       <c r="G16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="I22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
         <v>104</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" t="s">
         <v>114</v>
-      </c>
-      <c r="I19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1819,252 +1768,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F3" s="14" t="s">
-        <v>154</v>
+      <c r="F3" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="28"/>
+      <c r="F4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="27"/>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="16">
+        <v>30</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="19"/>
+      <c r="F5" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="18"/>
+      <c r="C6" s="20">
+        <v>20</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="H6" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="18">
+        <v>30</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19"/>
+      <c r="H7" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="18"/>
+      <c r="C8" s="20">
+        <v>20</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="H8" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="17">
+      <c r="J8" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="18">
         <v>30</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
-      <c r="F5" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="21">
-        <v>20</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="H6" s="14" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="20">
+        <v>30</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="H10" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="18">
+        <v>30</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="19"/>
+      <c r="H11" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="18"/>
+      <c r="C12" s="20">
+        <v>40</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="H12" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="18">
+        <v>40</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="18"/>
+      <c r="C14" s="20">
+        <v>40</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="H14" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="J6" s="14" t="s">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="18">
+        <v>40</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="H15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20">
+        <v>40</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="18">
+        <v>40</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20">
+        <v>40</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="H18" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="19">
-        <v>30</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="20"/>
-      <c r="H7" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="P7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
-      <c r="C8" s="21">
-        <v>20</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="H8" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19">
-        <v>30</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="21">
-        <v>30</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="H10" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="19">
-        <v>30</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20"/>
-      <c r="H11" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
-      <c r="C12" s="21">
-        <v>40</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="H12" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="19">
-        <v>40</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="20"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="21">
-        <v>40</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="H14" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="19">
-        <v>40</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="H15" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="19"/>
-      <c r="C16" s="21">
-        <v>40</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="19">
-        <v>40</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="21">
-        <v>40</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="H18" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="21">
         <v>40</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="20"/>
-      <c r="H19" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>153</v>
+      <c r="C19" s="22"/>
+      <c r="D19" s="19"/>
+      <c r="H19" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H20" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>140</v>
+      <c r="H20" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2074,4 +2023,92 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>